<commit_message>
corrigindo as funções pr, rk, vdw
</commit_message>
<xml_diff>
--- a/resultados.xlsx
+++ b/resultados.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,20 +436,25 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>Substância</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>Modelo</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Fase</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Volume Molar (cm³/mol)</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Massa Específica (g/cm³)</t>
         </is>
@@ -458,37 +463,24 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>VDW</t>
+          <t>Cloreto de Metila</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Líquido</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
-        <v>1766.4515</v>
+          <t>PR</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Vapor</t>
+        </is>
       </c>
       <c r="D2" t="n">
-        <v>0.028582</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>VDW</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Vapor</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>1766.4516</v>
-      </c>
-      <c r="D3" t="n">
-        <v>0.028582</v>
+        <v>2019.1856</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0.00099</v>
       </c>
     </row>
   </sheetData>

</xml_diff>